<commit_message>
refactor: enhance admin seeding logic with upsert; improve address handling and logging; hash passwords
</commit_message>
<xml_diff>
--- a/src/storage/assets/DoctorsLoginDetails.xlsx
+++ b/src/storage/assets/DoctorsLoginDetails.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\navin.kumar\Desktop\alineahealth all\hdfc-agro\src\storage\assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A5D148DE-7E4F-40A0-8E3C-74BFBA6463C1}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{47018F39-961C-48E6-A3B6-67F492735F7D}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="19200" windowHeight="6930" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="347" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="299" uniqueCount="149">
   <si>
     <t>ContactId</t>
   </si>
@@ -143,9 +143,6 @@
     <t>Ambekar</t>
   </si>
   <si>
-    <t>DF71DA78D17E24AC2B42E6232B12DC77</t>
-  </si>
-  <si>
     <t>Y</t>
   </si>
   <si>
@@ -465,69 +462,6 @@
   </si>
   <si>
     <t>DrMinakshi.Rathod@yopmail.com</t>
-  </si>
-  <si>
-    <t>Tajpur Road,,Samastipur</t>
-  </si>
-  <si>
-    <t>SAMASTIPUR</t>
-  </si>
-  <si>
-    <t>Bihar</t>
-  </si>
-  <si>
-    <t>848 101</t>
-  </si>
-  <si>
-    <t xml:space="preserve">098350 40714 / 222103                             </t>
-  </si>
-  <si>
-    <t>Opp.S.T.Stand,At.Kankavli,</t>
-  </si>
-  <si>
-    <t>Kankavli</t>
-  </si>
-  <si>
-    <t>Maharashtra</t>
-  </si>
-  <si>
-    <t>suryakanttayshete@yahoo.com</t>
-  </si>
-  <si>
-    <t>1/7-1/16,Govardhan Aptts.</t>
-  </si>
-  <si>
-    <t>Baroda</t>
-  </si>
-  <si>
-    <t>Gujarat</t>
-  </si>
-  <si>
-    <t>390 018</t>
-  </si>
-  <si>
-    <t>1st Floor   Sheeetal Apts.,Dwalat marg</t>
-  </si>
-  <si>
-    <t>Mumbai</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28927730, 28937611                                </t>
-  </si>
-  <si>
-    <t xml:space="preserve">j_a_lalwani@hotmail.com                           </t>
-  </si>
-  <si>
-    <t>Shastri Market, Padav,,</t>
-  </si>
-  <si>
-    <t>Gwalior</t>
-  </si>
-  <si>
-    <t>Madhya Pradesh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Na                                                </t>
   </si>
   <si>
     <t>6811eeb6e3bd4f1a1d39ab11</t>
@@ -1084,8 +1018,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AH6"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" topLeftCell="K1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1095,7 +1029,7 @@
     <col min="3" max="3" width="21.90625" customWidth="1"/>
     <col min="4" max="4" width="13.26953125" customWidth="1"/>
     <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="19.36328125" customWidth="1"/>
+    <col min="6" max="6" width="31.36328125" customWidth="1"/>
     <col min="7" max="7" width="17.7265625" customWidth="1"/>
     <col min="8" max="8" width="17" customWidth="1"/>
     <col min="9" max="9" width="14.90625" customWidth="1"/>
@@ -1249,10 +1183,10 @@
         <v>37</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="J2">
         <v>3230128</v>
@@ -1263,8 +1197,8 @@
       <c r="M2" t="s">
         <v>35</v>
       </c>
-      <c r="N2" t="s">
-        <v>38</v>
+      <c r="N2">
+        <v>123456</v>
       </c>
       <c r="O2" s="1">
         <v>45743.277712731498</v>
@@ -1276,37 +1210,37 @@
         <v>1</v>
       </c>
       <c r="R2" t="s">
+        <v>38</v>
+      </c>
+      <c r="S2" t="s">
+        <v>38</v>
+      </c>
+      <c r="T2" t="s">
         <v>39</v>
       </c>
-      <c r="S2" t="s">
+      <c r="U2" t="s">
+        <v>38</v>
+      </c>
+      <c r="V2" t="s">
+        <v>38</v>
+      </c>
+      <c r="W2" t="s">
         <v>39</v>
       </c>
-      <c r="T2" t="s">
-        <v>40</v>
-      </c>
-      <c r="U2" t="s">
+      <c r="X2" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y2" t="s">
         <v>39</v>
       </c>
-      <c r="V2" t="s">
-        <v>39</v>
-      </c>
-      <c r="W2" t="s">
-        <v>40</v>
-      </c>
-      <c r="X2" t="s">
+      <c r="Z2" t="s">
         <v>41</v>
       </c>
-      <c r="Y2" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z2" t="s">
+      <c r="AA2" t="s">
         <v>42</v>
       </c>
-      <c r="AA2" t="s">
+      <c r="AB2" t="s">
         <v>43</v>
-      </c>
-      <c r="AB2" t="s">
-        <v>44</v>
       </c>
       <c r="AC2" s="1">
         <v>45752.3299786227</v>
@@ -1341,19 +1275,19 @@
         <v>1</v>
       </c>
       <c r="E3" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" t="s">
         <v>45</v>
-      </c>
-      <c r="F3" t="s">
-        <v>46</v>
       </c>
       <c r="G3" t="s">
         <v>37</v>
       </c>
       <c r="H3" s="2" t="s">
-        <v>169</v>
+        <v>147</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="J3">
         <v>3231125</v>
@@ -1362,10 +1296,10 @@
         <v>1</v>
       </c>
       <c r="M3" t="s">
-        <v>45</v>
-      </c>
-      <c r="N3" t="s">
-        <v>38</v>
+        <v>44</v>
+      </c>
+      <c r="N3">
+        <v>123456</v>
       </c>
       <c r="O3" s="1">
         <v>45748.782214236096</v>
@@ -1377,40 +1311,40 @@
         <v>1</v>
       </c>
       <c r="R3" t="s">
+        <v>38</v>
+      </c>
+      <c r="S3" t="s">
+        <v>38</v>
+      </c>
+      <c r="T3" t="s">
         <v>39</v>
       </c>
-      <c r="S3" t="s">
+      <c r="U3" t="s">
+        <v>38</v>
+      </c>
+      <c r="V3" t="s">
+        <v>38</v>
+      </c>
+      <c r="W3" t="s">
         <v>39</v>
       </c>
-      <c r="T3" t="s">
-        <v>40</v>
-      </c>
-      <c r="U3" t="s">
+      <c r="X3" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y3" t="s">
         <v>39</v>
       </c>
-      <c r="V3" t="s">
-        <v>39</v>
-      </c>
-      <c r="W3" t="s">
-        <v>40</v>
-      </c>
-      <c r="X3" t="s">
+      <c r="Z3" t="s">
         <v>41</v>
       </c>
-      <c r="Y3" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z3" t="s">
+      <c r="AA3" t="s">
         <v>42</v>
       </c>
-      <c r="AA3" t="s">
+      <c r="AB3" t="s">
         <v>43</v>
       </c>
-      <c r="AB3" t="s">
-        <v>44</v>
-      </c>
       <c r="AC3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AD3">
         <v>0</v>
@@ -1425,7 +1359,7 @@
         <v>0</v>
       </c>
       <c r="AH3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:34">
@@ -1442,19 +1376,19 @@
         <v>1</v>
       </c>
       <c r="E4" t="s">
+        <v>46</v>
+      </c>
+      <c r="F4" t="s">
         <v>47</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
         <v>48</v>
       </c>
-      <c r="G4" t="s">
-        <v>49</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>170</v>
+        <v>148</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="J4">
         <v>3231126</v>
@@ -1463,10 +1397,10 @@
         <v>1</v>
       </c>
       <c r="M4" t="s">
-        <v>47</v>
-      </c>
-      <c r="N4" t="s">
-        <v>38</v>
+        <v>46</v>
+      </c>
+      <c r="N4">
+        <v>123456</v>
       </c>
       <c r="O4" s="1">
         <v>45748.797759027802</v>
@@ -1478,40 +1412,40 @@
         <v>1</v>
       </c>
       <c r="R4" t="s">
+        <v>38</v>
+      </c>
+      <c r="S4" t="s">
+        <v>38</v>
+      </c>
+      <c r="T4" t="s">
         <v>39</v>
       </c>
-      <c r="S4" t="s">
+      <c r="U4" t="s">
+        <v>38</v>
+      </c>
+      <c r="V4" t="s">
+        <v>38</v>
+      </c>
+      <c r="W4" t="s">
         <v>39</v>
       </c>
-      <c r="T4" t="s">
-        <v>40</v>
-      </c>
-      <c r="U4" t="s">
+      <c r="X4" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y4" t="s">
         <v>39</v>
       </c>
-      <c r="V4" t="s">
-        <v>39</v>
-      </c>
-      <c r="W4" t="s">
-        <v>40</v>
-      </c>
-      <c r="X4" t="s">
+      <c r="Z4" t="s">
         <v>41</v>
       </c>
-      <c r="Y4" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z4" t="s">
+      <c r="AA4" t="s">
         <v>42</v>
       </c>
-      <c r="AA4" t="s">
+      <c r="AB4" t="s">
         <v>43</v>
       </c>
-      <c r="AB4" t="s">
-        <v>44</v>
-      </c>
       <c r="AC4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AD4">
         <v>0</v>
@@ -1543,19 +1477,19 @@
         <v>1</v>
       </c>
       <c r="E5" t="s">
+        <v>49</v>
+      </c>
+      <c r="F5" t="s">
         <v>50</v>
       </c>
-      <c r="F5" t="s">
+      <c r="G5" t="s">
         <v>51</v>
       </c>
-      <c r="G5" t="s">
-        <v>52</v>
-      </c>
       <c r="H5" s="2" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="J5">
         <v>3231316</v>
@@ -1564,10 +1498,10 @@
         <v>1</v>
       </c>
       <c r="M5" t="s">
-        <v>50</v>
-      </c>
-      <c r="N5" t="s">
-        <v>38</v>
+        <v>49</v>
+      </c>
+      <c r="N5">
+        <v>123456</v>
       </c>
       <c r="O5" s="1">
         <v>45750.831765972202</v>
@@ -1579,40 +1513,40 @@
         <v>1</v>
       </c>
       <c r="R5" t="s">
+        <v>38</v>
+      </c>
+      <c r="S5" t="s">
+        <v>38</v>
+      </c>
+      <c r="T5" t="s">
         <v>39</v>
       </c>
-      <c r="S5" t="s">
+      <c r="U5" t="s">
+        <v>38</v>
+      </c>
+      <c r="V5" t="s">
+        <v>38</v>
+      </c>
+      <c r="W5" t="s">
         <v>39</v>
       </c>
-      <c r="T5" t="s">
-        <v>40</v>
-      </c>
-      <c r="U5" t="s">
+      <c r="X5" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y5" t="s">
         <v>39</v>
       </c>
-      <c r="V5" t="s">
-        <v>39</v>
-      </c>
-      <c r="W5" t="s">
-        <v>40</v>
-      </c>
-      <c r="X5" t="s">
+      <c r="Z5" t="s">
         <v>41</v>
       </c>
-      <c r="Y5" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z5" t="s">
+      <c r="AA5" t="s">
         <v>42</v>
       </c>
-      <c r="AA5" t="s">
+      <c r="AB5" t="s">
         <v>43</v>
       </c>
-      <c r="AB5" t="s">
-        <v>44</v>
-      </c>
       <c r="AC5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AD5">
         <v>0</v>
@@ -1644,19 +1578,19 @@
         <v>1</v>
       </c>
       <c r="E6" t="s">
+        <v>52</v>
+      </c>
+      <c r="F6" t="s">
         <v>53</v>
       </c>
-      <c r="F6" t="s">
+      <c r="G6" t="s">
         <v>54</v>
       </c>
-      <c r="G6" t="s">
-        <v>55</v>
-      </c>
       <c r="H6" s="2" t="s">
-        <v>167</v>
+        <v>145</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>168</v>
+        <v>146</v>
       </c>
       <c r="J6">
         <v>3231328</v>
@@ -1665,10 +1599,10 @@
         <v>1</v>
       </c>
       <c r="M6" t="s">
-        <v>53</v>
-      </c>
-      <c r="N6" t="s">
-        <v>38</v>
+        <v>52</v>
+      </c>
+      <c r="N6">
+        <v>123456</v>
       </c>
       <c r="O6" s="1">
         <v>45751.696271956003</v>
@@ -1680,40 +1614,40 @@
         <v>1</v>
       </c>
       <c r="R6" t="s">
+        <v>38</v>
+      </c>
+      <c r="S6" t="s">
+        <v>38</v>
+      </c>
+      <c r="T6" t="s">
         <v>39</v>
       </c>
-      <c r="S6" t="s">
+      <c r="U6" t="s">
+        <v>38</v>
+      </c>
+      <c r="V6" t="s">
+        <v>38</v>
+      </c>
+      <c r="W6" t="s">
         <v>39</v>
       </c>
-      <c r="T6" t="s">
-        <v>40</v>
-      </c>
-      <c r="U6" t="s">
+      <c r="X6" t="s">
+        <v>40</v>
+      </c>
+      <c r="Y6" t="s">
         <v>39</v>
       </c>
-      <c r="V6" t="s">
-        <v>39</v>
-      </c>
-      <c r="W6" t="s">
-        <v>40</v>
-      </c>
-      <c r="X6" t="s">
+      <c r="Z6" t="s">
         <v>41</v>
       </c>
-      <c r="Y6" t="s">
-        <v>40</v>
-      </c>
-      <c r="Z6" t="s">
+      <c r="AA6" t="s">
         <v>42</v>
       </c>
-      <c r="AA6" t="s">
+      <c r="AB6" t="s">
         <v>43</v>
       </c>
-      <c r="AB6" t="s">
-        <v>44</v>
-      </c>
       <c r="AC6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="AD6">
         <v>0</v>
@@ -1740,8 +1674,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:K18"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="N7" sqref="N7"/>
+    <sheetView topLeftCell="C1" workbookViewId="0">
+      <selection activeCell="I7" sqref="I7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.7265625" defaultRowHeight="14.5"/>
@@ -1757,37 +1691,37 @@
   <sheetData>
     <row r="1" spans="1:11">
       <c r="A1" t="s">
+        <v>55</v>
+      </c>
+      <c r="B1" t="s">
         <v>56</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>57</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>58</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>59</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>60</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>61</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>62</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>63</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>64</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>65</v>
-      </c>
-      <c r="K1" t="s">
-        <v>66</v>
       </c>
     </row>
     <row r="2" spans="1:11">
@@ -1795,19 +1729,19 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="C2">
         <v>739604</v>
       </c>
       <c r="D2" t="s">
+        <v>67</v>
+      </c>
+      <c r="F2" t="s">
         <v>68</v>
       </c>
-      <c r="F2" t="s">
-        <v>69</v>
-      </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2">
         <v>1</v>
@@ -1816,10 +1750,10 @@
         <v>45719.632253090298</v>
       </c>
       <c r="J2" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="3" spans="1:11">
@@ -1827,7 +1761,7 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C3">
         <v>739593</v>
@@ -1836,10 +1770,10 @@
         <v>64682</v>
       </c>
       <c r="F3" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3">
         <v>1</v>
@@ -1848,10 +1782,10 @@
         <v>45719.632253090298</v>
       </c>
       <c r="J3" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="4" spans="1:11">
@@ -1859,7 +1793,7 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C4">
         <v>739595</v>
@@ -1868,10 +1802,10 @@
         <v>67149</v>
       </c>
       <c r="F4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="G4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H4">
         <v>1</v>
@@ -1880,10 +1814,10 @@
         <v>45719.632253090298</v>
       </c>
       <c r="J4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:11">
@@ -1891,7 +1825,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C5">
         <v>739594</v>
@@ -1900,10 +1834,10 @@
         <v>32801</v>
       </c>
       <c r="F5" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5">
         <v>1</v>
@@ -1912,10 +1846,10 @@
         <v>45719.632253090298</v>
       </c>
       <c r="J5" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K5" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="6" spans="1:11">
@@ -1923,7 +1857,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C6">
         <v>739584</v>
@@ -1932,10 +1866,10 @@
         <v>2234</v>
       </c>
       <c r="F6" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H6">
         <v>1</v>
@@ -1944,10 +1878,10 @@
         <v>45719.632253090298</v>
       </c>
       <c r="J6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K6" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="7" spans="1:11">
@@ -1955,7 +1889,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="C7">
         <v>739585</v>
@@ -1964,10 +1898,10 @@
         <v>69257</v>
       </c>
       <c r="F7" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="G7" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H7">
         <v>1</v>
@@ -1976,10 +1910,10 @@
         <v>45719.632253090298</v>
       </c>
       <c r="J7" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K7" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="8" spans="1:11">
@@ -1987,19 +1921,19 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="C8">
         <v>739586</v>
       </c>
       <c r="D8" t="s">
+        <v>82</v>
+      </c>
+      <c r="F8" t="s">
         <v>83</v>
       </c>
-      <c r="F8" t="s">
-        <v>84</v>
-      </c>
       <c r="G8" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H8">
         <v>1</v>
@@ -2008,10 +1942,10 @@
         <v>45719.632253090298</v>
       </c>
       <c r="J8" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K8" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="9" spans="1:11">
@@ -2019,19 +1953,19 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="C9">
         <v>739587</v>
       </c>
       <c r="D9" t="s">
+        <v>85</v>
+      </c>
+      <c r="F9" t="s">
         <v>86</v>
       </c>
-      <c r="F9" t="s">
-        <v>87</v>
-      </c>
       <c r="G9" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H9">
         <v>1</v>
@@ -2040,10 +1974,10 @@
         <v>45719.632253090298</v>
       </c>
       <c r="J9" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K9" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="10" spans="1:11">
@@ -2051,7 +1985,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="C10">
         <v>739588</v>
@@ -2060,10 +1994,10 @@
         <v>2247</v>
       </c>
       <c r="F10" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="G10" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H10">
         <v>1</v>
@@ -2072,10 +2006,10 @@
         <v>45719.632253090298</v>
       </c>
       <c r="J10" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K10" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="11" spans="1:11">
@@ -2083,19 +2017,19 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="C11">
         <v>739589</v>
       </c>
       <c r="D11" t="s">
+        <v>90</v>
+      </c>
+      <c r="F11" t="s">
         <v>91</v>
       </c>
-      <c r="F11" t="s">
-        <v>92</v>
-      </c>
       <c r="G11" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H11">
         <v>1</v>
@@ -2104,10 +2038,10 @@
         <v>45719.632253090298</v>
       </c>
       <c r="J11" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="12" spans="1:11">
@@ -2115,7 +2049,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="C12">
         <v>739590</v>
@@ -2124,10 +2058,10 @@
         <v>30928</v>
       </c>
       <c r="F12" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="G12" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H12">
         <v>1</v>
@@ -2136,10 +2070,10 @@
         <v>45719.632253090298</v>
       </c>
       <c r="J12" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K12" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="13" spans="1:11">
@@ -2147,19 +2081,19 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="C13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="D13">
         <v>32184</v>
       </c>
       <c r="F13" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="G13" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H13">
         <v>1</v>
@@ -2168,10 +2102,10 @@
         <v>45719.632253090298</v>
       </c>
       <c r="J13" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K13" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="14" spans="1:11">
@@ -2179,7 +2113,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="C14">
         <v>739591</v>
@@ -2188,10 +2122,10 @@
         <v>30626</v>
       </c>
       <c r="F14" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="G14" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H14">
         <v>1</v>
@@ -2200,10 +2134,10 @@
         <v>45719.632253090298</v>
       </c>
       <c r="J14" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K14" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="15" spans="1:11">
@@ -2211,22 +2145,22 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C15">
         <v>738410</v>
       </c>
       <c r="D15" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="E15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G15" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H15">
         <v>1</v>
@@ -2235,10 +2169,10 @@
         <v>45729.542988159701</v>
       </c>
       <c r="J15" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K15" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="16" spans="1:11">
@@ -2246,22 +2180,22 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="C16">
         <v>739406</v>
       </c>
       <c r="D16" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="E16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G16" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H16">
         <v>1</v>
@@ -2270,10 +2204,10 @@
         <v>45749.972643831003</v>
       </c>
       <c r="J16" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K16" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="17" spans="1:11">
@@ -2281,7 +2215,7 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="C17">
         <v>739407</v>
@@ -2290,13 +2224,13 @@
         <v>13719301</v>
       </c>
       <c r="E17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="F17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="G17" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H17">
         <v>1</v>
@@ -2305,10 +2239,10 @@
         <v>45766.467095601904</v>
       </c>
       <c r="J17" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="K17" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="18" spans="1:11">
@@ -2316,7 +2250,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="C18">
         <v>742168</v>
@@ -2325,10 +2259,10 @@
         <v>6167</v>
       </c>
       <c r="F18" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="G18" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H18">
         <v>1</v>
@@ -2337,10 +2271,10 @@
         <v>45770.471917939802</v>
       </c>
       <c r="J18" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="K18" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
   </sheetData>
@@ -2352,52 +2286,55 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3DAE457B-75E2-433C-BCC9-0A9F3B22AF3C}">
   <dimension ref="A1:O11"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+    <sheetView topLeftCell="F1" workbookViewId="0">
+      <selection activeCell="L12" sqref="L12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5"/>
   <cols>
-    <col min="2" max="2" width="26" customWidth="1"/>
+    <col min="1" max="1" width="25.54296875" customWidth="1"/>
+    <col min="2" max="2" width="35.1796875" customWidth="1"/>
     <col min="3" max="3" width="17.7265625" customWidth="1"/>
     <col min="4" max="4" width="14.6328125" customWidth="1"/>
+    <col min="5" max="5" width="19.81640625" customWidth="1"/>
     <col min="7" max="7" width="11" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="22.1796875" customWidth="1"/>
     <col min="10" max="10" width="33.90625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:15">
       <c r="A1" t="s">
+        <v>106</v>
+      </c>
+      <c r="B1" t="s">
         <v>107</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>108</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>109</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>110</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>111</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>112</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>113</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>114</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>115</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>116</v>
-      </c>
-      <c r="K1" t="s">
-        <v>117</v>
       </c>
       <c r="L1" t="s">
         <v>15</v>
@@ -2406,10 +2343,10 @@
         <v>16</v>
       </c>
       <c r="N1" t="s">
+        <v>117</v>
+      </c>
+      <c r="O1" t="s">
         <v>118</v>
-      </c>
-      <c r="O1" t="s">
-        <v>119</v>
       </c>
     </row>
     <row r="2" spans="1:15">
@@ -2417,22 +2354,22 @@
         <v>3230128</v>
       </c>
       <c r="B2" t="s">
+        <v>119</v>
+      </c>
+      <c r="C2" t="s">
         <v>120</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
+        <v>40</v>
+      </c>
+      <c r="E2" t="s">
         <v>121</v>
       </c>
-      <c r="D2" t="s">
-        <v>41</v>
-      </c>
-      <c r="E2" t="s">
+      <c r="F2" t="s">
         <v>122</v>
       </c>
-      <c r="F2" t="s">
-        <v>123</v>
-      </c>
       <c r="G2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H2">
         <v>23514572</v>
@@ -2441,7 +2378,7 @@
         <v>23517044</v>
       </c>
       <c r="J2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="K2" s="1">
         <v>38628.463159722225</v>
@@ -2453,10 +2390,10 @@
         <v>0</v>
       </c>
       <c r="N2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="3" spans="1:15">
@@ -2464,31 +2401,31 @@
         <v>3231125</v>
       </c>
       <c r="B3" t="s">
+        <v>124</v>
+      </c>
+      <c r="C3" t="s">
         <v>125</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
+        <v>40</v>
+      </c>
+      <c r="E3" t="s">
         <v>126</v>
-      </c>
-      <c r="D3" t="s">
-        <v>41</v>
-      </c>
-      <c r="E3" t="s">
-        <v>127</v>
       </c>
       <c r="F3">
         <v>605001</v>
       </c>
       <c r="G3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H3" t="s">
+        <v>127</v>
+      </c>
+      <c r="I3" t="s">
         <v>128</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>129</v>
-      </c>
-      <c r="J3" t="s">
-        <v>130</v>
       </c>
       <c r="K3" s="1">
         <v>38628.463159722225</v>
@@ -2500,10 +2437,10 @@
         <v>0</v>
       </c>
       <c r="N3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="4" spans="1:15">
@@ -2511,31 +2448,31 @@
         <v>3231126</v>
       </c>
       <c r="B4" t="s">
+        <v>130</v>
+      </c>
+      <c r="C4" t="s">
         <v>131</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
+        <v>40</v>
+      </c>
+      <c r="E4" t="s">
         <v>132</v>
       </c>
-      <c r="D4" t="s">
-        <v>41</v>
-      </c>
-      <c r="E4" t="s">
+      <c r="F4" t="s">
         <v>133</v>
       </c>
-      <c r="F4" t="s">
+      <c r="G4" t="s">
+        <v>40</v>
+      </c>
+      <c r="H4" t="s">
         <v>134</v>
       </c>
-      <c r="G4" t="s">
-        <v>41</v>
-      </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>135</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>136</v>
-      </c>
-      <c r="J4" t="s">
-        <v>137</v>
       </c>
       <c r="K4" s="1">
         <v>38628.463159722225</v>
@@ -2547,10 +2484,10 @@
         <v>0</v>
       </c>
       <c r="N4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O4" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="5" spans="1:15">
@@ -2558,31 +2495,31 @@
         <v>3231316</v>
       </c>
       <c r="B5" t="s">
+        <v>137</v>
+      </c>
+      <c r="C5" t="s">
         <v>138</v>
       </c>
-      <c r="C5" t="s">
+      <c r="D5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E5" t="s">
+        <v>132</v>
+      </c>
+      <c r="F5" t="s">
         <v>139</v>
       </c>
-      <c r="D5" t="s">
-        <v>41</v>
-      </c>
-      <c r="E5" t="s">
-        <v>133</v>
-      </c>
-      <c r="F5" t="s">
-        <v>140</v>
-      </c>
       <c r="G5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H5">
         <v>270436</v>
       </c>
       <c r="I5" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J5" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="K5" s="1">
         <v>38628.463159722225</v>
@@ -2594,42 +2531,42 @@
         <v>0</v>
       </c>
       <c r="N5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O5" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="6" spans="1:15">
       <c r="A6">
-        <v>3231320</v>
+        <v>3231328</v>
       </c>
       <c r="B6" t="s">
+        <v>141</v>
+      </c>
+      <c r="C6" t="s">
         <v>142</v>
       </c>
-      <c r="C6" t="s">
+      <c r="D6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E6" t="s">
         <v>143</v>
-      </c>
-      <c r="D6" t="s">
-        <v>41</v>
-      </c>
-      <c r="E6" t="s">
-        <v>144</v>
       </c>
       <c r="F6">
         <v>400066</v>
       </c>
       <c r="G6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="H6">
         <v>55767442</v>
       </c>
       <c r="I6" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="J6" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="K6" s="1">
         <v>38628.463159722225</v>
@@ -2641,246 +2578,35 @@
         <v>0</v>
       </c>
       <c r="N6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="O6" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="7" spans="1:15">
-      <c r="A7">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
-        <v>146</v>
-      </c>
-      <c r="C7" t="s">
-        <v>147</v>
-      </c>
-      <c r="D7" t="s">
-        <v>41</v>
-      </c>
-      <c r="E7" t="s">
-        <v>148</v>
-      </c>
-      <c r="F7" t="s">
-        <v>149</v>
-      </c>
-      <c r="G7">
-        <v>9835040714</v>
-      </c>
-      <c r="H7" t="s">
-        <v>150</v>
-      </c>
-      <c r="I7" t="s">
-        <v>41</v>
-      </c>
-      <c r="J7" t="s">
-        <v>41</v>
-      </c>
-      <c r="K7" s="1">
-        <v>38628.463159722225</v>
-      </c>
-      <c r="L7" s="1">
-        <v>40561.417360729167</v>
-      </c>
-      <c r="M7">
+      <c r="B7">
+        <f>D7</f>
         <v>0</v>
       </c>
-      <c r="N7" t="s">
-        <v>41</v>
-      </c>
-      <c r="O7" t="s">
-        <v>41</v>
-      </c>
+      <c r="K7" s="1"/>
+      <c r="L7" s="1"/>
     </row>
     <row r="8" spans="1:15">
-      <c r="A8">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
-        <v>151</v>
-      </c>
-      <c r="C8" t="s">
-        <v>152</v>
-      </c>
-      <c r="D8" t="s">
-        <v>41</v>
-      </c>
-      <c r="E8" t="s">
-        <v>153</v>
-      </c>
-      <c r="F8">
-        <v>416602</v>
-      </c>
-      <c r="G8">
-        <v>9822583735</v>
-      </c>
-      <c r="H8">
-        <v>230482</v>
-      </c>
-      <c r="I8">
-        <v>232184</v>
-      </c>
-      <c r="J8" t="s">
-        <v>154</v>
-      </c>
-      <c r="K8" s="1">
-        <v>38628.463159722225</v>
-      </c>
-      <c r="L8" s="1">
-        <v>45572.666878240743</v>
-      </c>
-      <c r="M8">
-        <v>1</v>
-      </c>
-      <c r="N8" t="s">
-        <v>41</v>
-      </c>
-      <c r="O8" t="s">
-        <v>41</v>
-      </c>
+      <c r="K8" s="1"/>
+      <c r="L8" s="1"/>
     </row>
     <row r="9" spans="1:15">
-      <c r="A9">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
-        <v>155</v>
-      </c>
-      <c r="C9" t="s">
-        <v>156</v>
-      </c>
-      <c r="D9" t="s">
-        <v>41</v>
-      </c>
-      <c r="E9" t="s">
-        <v>157</v>
-      </c>
-      <c r="F9" t="s">
-        <v>158</v>
-      </c>
-      <c r="G9">
-        <v>9824047127</v>
-      </c>
-      <c r="H9">
-        <v>2480034</v>
-      </c>
-      <c r="I9" t="s">
-        <v>136</v>
-      </c>
-      <c r="J9" t="s">
-        <v>136</v>
-      </c>
-      <c r="K9" s="1">
-        <v>38628.463159722225</v>
-      </c>
-      <c r="L9" s="1">
-        <v>40561.417221840275</v>
-      </c>
-      <c r="M9">
-        <v>0</v>
-      </c>
-      <c r="N9" t="s">
-        <v>41</v>
-      </c>
-      <c r="O9" t="s">
-        <v>41</v>
-      </c>
+      <c r="K9" s="1"/>
+      <c r="L9" s="1"/>
     </row>
     <row r="10" spans="1:15">
-      <c r="A10">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
-        <v>159</v>
-      </c>
-      <c r="C10" t="s">
-        <v>160</v>
-      </c>
-      <c r="D10" t="s">
-        <v>41</v>
-      </c>
-      <c r="E10" t="s">
-        <v>153</v>
-      </c>
-      <c r="F10">
-        <v>400066</v>
-      </c>
-      <c r="G10">
-        <v>9820081207</v>
-      </c>
-      <c r="H10" t="s">
-        <v>161</v>
-      </c>
-      <c r="I10" t="s">
-        <v>136</v>
-      </c>
-      <c r="J10" t="s">
-        <v>162</v>
-      </c>
-      <c r="K10" s="1">
-        <v>38628.463159722225</v>
-      </c>
-      <c r="L10" s="1">
-        <v>41166.583637696756</v>
-      </c>
-      <c r="M10">
-        <v>0</v>
-      </c>
-      <c r="N10" t="s">
-        <v>41</v>
-      </c>
-      <c r="O10" t="s">
-        <v>41</v>
-      </c>
+      <c r="K10" s="1"/>
+      <c r="L10" s="1"/>
     </row>
     <row r="11" spans="1:15">
-      <c r="A11">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
-        <v>163</v>
-      </c>
-      <c r="C11" t="s">
-        <v>164</v>
-      </c>
-      <c r="D11" t="s">
-        <v>41</v>
-      </c>
-      <c r="E11" t="s">
-        <v>165</v>
-      </c>
-      <c r="F11">
-        <v>474001</v>
-      </c>
-      <c r="G11" t="s">
-        <v>41</v>
-      </c>
-      <c r="H11">
-        <v>5013353</v>
-      </c>
-      <c r="I11">
-        <v>5013333</v>
-      </c>
-      <c r="J11" t="s">
-        <v>166</v>
-      </c>
-      <c r="K11" s="1">
-        <v>38628.463159722225</v>
-      </c>
-      <c r="L11" s="1">
-        <v>40561.417314583334</v>
-      </c>
-      <c r="M11">
-        <v>0</v>
-      </c>
-      <c r="N11" t="s">
-        <v>41</v>
-      </c>
-      <c r="O11" t="s">
-        <v>41</v>
-      </c>
+      <c r="K11" s="1"/>
+      <c r="L11" s="1"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>